<commit_message>
Revert "Merge branch 'master' into xh"
This reverts commit 4ee4ca2b58425a3915f9accca60a55bb08137b66, reversing
changes made to d8befbc8655e1c9aa339a416920037ac1b4f2d3b.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -223,10 +223,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -255,14 +255,6 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -304,57 +296,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -378,6 +319,58 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,9 +387,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -423,13 +423,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,6 +513,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -465,7 +561,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -478,126 +598,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -689,17 +689,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -719,15 +728,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -743,26 +743,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -794,10 +794,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -806,133 +806,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1308,8 +1308,8 @@
   <sheetPr/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E17 E18 E19 E20 E22 E23 E26 E27 E28 E30 E32 E34 E36 E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1586,7 +1586,9 @@
         <v>23</v>
       </c>
       <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="8"/>
@@ -1704,7 +1706,9 @@
         <v>23</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="8"/>
@@ -1724,7 +1728,9 @@
         <v>8</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="8"/>
@@ -1746,7 +1752,9 @@
         <v>8</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="11"/>
+      <c r="E19" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F19" s="11"/>
       <c r="G19" s="11"/>
       <c r="H19" s="13"/>
@@ -1768,7 +1776,9 @@
         <v>8</v>
       </c>
       <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="8"/>
@@ -1812,7 +1822,9 @@
         <v>37</v>
       </c>
       <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="8"/>
@@ -1832,7 +1844,9 @@
         <v>8</v>
       </c>
       <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="8"/>
@@ -1902,7 +1916,9 @@
       <c r="D26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="8"/>
@@ -1922,7 +1938,9 @@
         <v>8</v>
       </c>
       <c r="D27" s="3"/>
-      <c r="E27" s="4"/>
+      <c r="E27" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="8"/>
@@ -1942,7 +1960,9 @@
         <v>37</v>
       </c>
       <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
+      <c r="E28" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="8"/>
@@ -1990,7 +2010,9 @@
       <c r="D30" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="8"/>
@@ -2036,7 +2058,9 @@
       <c r="D32" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="8"/>
@@ -2084,7 +2108,9 @@
       <c r="D34" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="11"/>
+      <c r="E34" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
       <c r="H34" s="13"/>
@@ -2132,7 +2158,9 @@
       <c r="D36" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="E36" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="8"/>
@@ -2180,7 +2208,9 @@
       <c r="D38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E38" s="4"/>
+      <c r="E38" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="15"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' into czx"
This reverts commit bd9072a6648f6c11cef5bf941456d0ed267385bd, reversing
changes made to aae1ddbdca48f3e271625a92dc0c6d45e82a6865.
</commit_message>
<xml_diff>
--- a/作业完成情况汇总.xlsx
+++ b/作业完成情况汇总.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13065"/>
+    <workbookView windowWidth="28695" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70">
   <si>
     <t>WHJ171103班晚自习作业完成情况汇总表</t>
   </si>
@@ -186,9 +186,6 @@
   </si>
   <si>
     <t>在复习前几天的知识点</t>
-  </si>
-  <si>
-    <t>完成1</t>
   </si>
   <si>
     <t>严宇丛</t>
@@ -235,10 +232,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -270,17 +267,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -291,15 +282,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -320,11 +343,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -336,39 +365,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -392,7 +390,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -400,17 +398,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -435,108 +432,174 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -550,72 +613,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,54 +670,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -744,11 +693,48 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -767,6 +753,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -775,10 +772,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -787,19 +784,19 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -808,112 +805,112 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1277,8 +1274,8 @@
   <sheetPr/>
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1479,7 +1476,9 @@
         <v>8</v>
       </c>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
@@ -1581,7 +1580,9 @@
       <c r="H12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
@@ -1686,8 +1687,12 @@
       <c r="G16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="H16" s="4">
+        <v>11111</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J16" s="4"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
@@ -1707,9 +1712,13 @@
         <v>8</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+      <c r="I17" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J17" s="4"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
@@ -1729,9 +1738,13 @@
         <v>8</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
@@ -1753,9 +1766,13 @@
         <v>8</v>
       </c>
       <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
+      <c r="G19" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
+      <c r="I19" s="9" t="s">
+        <v>8</v>
+      </c>
       <c r="J19" s="9"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
@@ -1875,9 +1892,13 @@
         <v>8</v>
       </c>
       <c r="F24" s="9"/>
-      <c r="G24" s="11"/>
+      <c r="G24" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="H24" s="9"/>
-      <c r="I24" s="11"/>
+      <c r="I24" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="J24" s="9"/>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
@@ -1901,7 +1922,9 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
+      <c r="I25" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J25" s="4"/>
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
@@ -1923,9 +1946,13 @@
         <v>8</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="G26" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J26" s="4"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
@@ -2023,7 +2050,9 @@
       <c r="H30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J30" s="4"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
@@ -2101,7 +2130,7 @@
         <v>56</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="13"/>
@@ -2114,13 +2143,13 @@
         <v>14</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="D34" s="11" t="s">
         <v>59</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>60</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>8</v>
@@ -2130,7 +2159,7 @@
         <v>8</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I34" s="9" t="s">
         <v>8</v>
@@ -2146,13 +2175,13 @@
         <v>16</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>12</v>
@@ -2174,13 +2203,13 @@
     <row r="36" ht="25" customHeight="1" spans="1:14">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>8</v>
@@ -2188,7 +2217,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
@@ -2200,13 +2229,13 @@
     <row r="37" ht="25" customHeight="1" spans="1:14">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>12</v>
@@ -2226,13 +2255,13 @@
     <row r="38" ht="25" customHeight="1" spans="1:14">
       <c r="A38" s="3"/>
       <c r="B38" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>8</v>
@@ -2240,7 +2269,9 @@
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
+      <c r="I38" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J38" s="4"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>

</xml_diff>